<commit_message>
Heading to V2.5.0, huge backup
</commit_message>
<xml_diff>
--- a/wordpress/wp-content/themes/bsawesome/inc/configurator/pricematrices.xlsx
+++ b/wordpress/wp-content/themes/bsawesome/inc/configurator/pricematrices.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\data\docker\volumes\DevKinsta\public\badspiegel\wp-content\themes\bsawesome\inc\configurator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\imabidin\badspiegel\wordpress\wp-content\themes\bsawesome\inc\configurator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAE9AE71-6274-4725-B375-E224CF008E3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6F113D1-DA25-47A7-9CE7-54BCB155A489}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2955" yWindow="2595" windowWidth="30555" windowHeight="15345" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3450" yWindow="3090" windowWidth="28770" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="defaults" sheetId="1" r:id="rId1"/>
@@ -2095,8 +2095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2287,7 +2287,7 @@
         <v>34</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C17" t="s">
         <v>35</v>
@@ -2343,7 +2343,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O448"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D74" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>